<commit_message>
done project (readme in italian)
</commit_message>
<xml_diff>
--- a/timetables/aida.xlsx
+++ b/timetables/aida.xlsx
@@ -488,51 +488,48 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 2B]
+          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1A]
+ &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H2 Bis, 5C]</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1A]
+ &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H2 Bis, 5C]</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1A]</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> &gt; NESSUNA LEZIONE</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> &gt; PROGRAMMAZIONE AVANZATA E PARALLELA [H3, 1B]</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> &gt; ALGEBRA LINEARE ED ELEMENTI DI GEOMETRIA [H3, 1A]
+ &gt; PROGRAMMAZIONE AVANZATA E PARALLELA [H3, 1B]</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> &gt; ALGEBRA LINEARE ED ELEMENTI DI GEOMETRIA [H3, 1A]
  &gt; ALGORITMI E STRUTTURE DATI [H2 Bis, 3B]
- &gt; SISTEMI COMPLESSI [H2 Bis, 2A MORIN]</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 2B]
- &gt; ALGORITMI E STRUTTURE DATI [H2 Bis, 3B]
- &gt; SISTEMI COMPLESSI [H2 Bis, 2A MORIN]</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 2B]
- &gt; ALGORITMI E STRUTTURE DATI [H3, 2A]
- &gt; SISTEMI COMPLESSI [H2 Bis, 2A MORIN]</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 2B]
- &gt; ALGORITMI E STRUTTURE DATI [H3, 2A]</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> &gt; PROGRAMMAZIONE AVANZATA E PARALLELA [H3, 2A]</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> &gt; PROGRAMMAZIONE AVANZATA E PARALLELA [H3, 2A]</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> &gt; ANALISI 1 [H2 Bis, 2A MORIN]
- &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H2 Bis, 5C]</t>
+ &gt; INTRODUZIONE AL MACHINE LEARNING [H3, 1B]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ANALISI 1 [H2 Bis, 2A MORIN]
- &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H2 Bis, 5C]</t>
+          <t xml:space="preserve"> &gt; ALGORITMI E STRUTTURE DATI [H2 Bis, 3B]
+ &gt; INTRODUZIONE AL MACHINE LEARNING [H3, 1B]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -549,50 +546,46 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ANALISI 1 [H2 Bis, 2A MORIN]
- &gt; PROGRAMMAZIONE AVANZATA E PARALLELA [H3, 2B]</t>
+          <t xml:space="preserve"> &gt; ANALISI 1 [H3, 1A]
+ &gt; PROGRAMMAZIONE AVANZATA E PARALLELA [H3, 2A]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ANALISI 1 [H2 Bis, 2A MORIN]
- &gt; PROGRAMMAZIONE AVANZATA E PARALLELA [H3, 2B]</t>
+          <t xml:space="preserve"> &gt; ANALISI 1 [H3, 1A]
+ &gt; PROGRAMMAZIONE AVANZATA E PARALLELA [H3, 2A]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ALGEBRA LINEARE ED ELEMENTI DI GEOMETRIA [H2 Bis, 2A MORIN]
- &gt; INFERENZA STATISTICA [H3, 1C]
- &gt; INTRODUZIONE AL MACHINE LEARNING [H2 Bis, 3B]</t>
+          <t xml:space="preserve"> &gt; ARCHITETTURE DEGLI ELABORATORI [H3, 2B]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ALGEBRA LINEARE ED ELEMENTI DI GEOMETRIA [H2 Bis, 2A MORIN]
- &gt; INFERENZA STATISTICA [H3, 1C]
- &gt; INTRODUZIONE AL MACHINE LEARNING [H2 Bis, 3B]</t>
+          <t xml:space="preserve"> &gt; ARCHITETTURE DEGLI ELABORATORI [H3, 2B]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H2 Bis, 4C]</t>
+          <t xml:space="preserve"> &gt; ARCHITETTURE DEGLI ELABORATORI [H3, 2B]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H2 Bis, 4C]</t>
+          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 2B]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; COMPUTABILITà, COMPLESSITà E LOGICA [H3, 1C]
- &gt; SISTEMI COMPLESSI [H3, 1A]</t>
+          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 2B]
+ &gt; ALGORITMI E STRUTTURE DATI [H3, 2A]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; COMPUTABILITà, COMPLESSITà E LOGICA [H3, 1C]
- &gt; SISTEMI COMPLESSI [H3, 1A]</t>
+          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 2B]
+ &gt; ALGORITMI E STRUTTURE DATI [H3, 2A]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -609,46 +602,44 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1A]</t>
+          <t xml:space="preserve"> &gt; SISTEMI COMPLESSI [H3, 1B]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1A]</t>
+          <t xml:space="preserve"> &gt; INFERENZA STATISTICA [H3, 1C]
+ &gt; SISTEMI COMPLESSI [H3, 1B]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1A]</t>
+          <t xml:space="preserve"> &gt; INFERENZA STATISTICA [H3, 1C]
+ &gt; SISTEMI COMPLESSI [H3, 1B]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H3, 2A]</t>
+          <t xml:space="preserve"> &gt; PROGRAMMAZIONE AVANZATA E PARALLELA [H3, 2A]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ALGEBRA LINEARE ED ELEMENTI DI GEOMETRIA [H2 Bis, 2A MORIN]
- &gt; ALGORITMI E STRUTTURE DATI [H3, 2B]
- &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H3, 2A]</t>
+          <t xml:space="preserve"> &gt; PROGRAMMAZIONE AVANZATA E PARALLELA [H3, 2A]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ALGEBRA LINEARE ED ELEMENTI DI GEOMETRIA [H2 Bis, 2A MORIN]
- &gt; ALGORITMI E STRUTTURE DATI [H3, 2B]
- &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H3, 2A]</t>
+          <t xml:space="preserve"> &gt; NESSUNA LEZIONE</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; NESSUNA LEZIONE</t>
+          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 2B]</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; NESSUNA LEZIONE</t>
+          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 2B]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -665,50 +656,50 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 2B]</t>
+          <t xml:space="preserve"> &gt; ALGORITMI E STRUTTURE DATI [H2 Bis, 2A MORIN]
+ &gt; SISTEMI COMPLESSI [H2 Bis, 3B]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 2B]</t>
+          <t xml:space="preserve"> &gt; ALGORITMI E STRUTTURE DATI [H2 Bis, 2A MORIN]
+ &gt; SISTEMI COMPLESSI [H2 Bis, 3B]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ARCHITETTURE DEGLI ELABORATORI [H3, 2B]</t>
+          <t xml:space="preserve"> &gt; ANALISI 1 [H3, 1B]
+ &gt; INFERENZA STATISTICA [H2 Bis, 2A MORIN]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ARCHITETTURE DEGLI ELABORATORI [H3, 2B]
- &gt; INFERENZA STATISTICA [H3, 2C]
- &gt; INTRODUZIONE AL MACHINE LEARNING [H2 Bis, 2A MORIN]</t>
+          <t xml:space="preserve"> &gt; ANALISI 1 [H3, 1B]
+ &gt; INFERENZA STATISTICA [H2 Bis, 2A MORIN]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ARCHITETTURE DEGLI ELABORATORI [H3, 2B]
- &gt; INFERENZA STATISTICA [H3, 2C]
- &gt; INTRODUZIONE AL MACHINE LEARNING [H2 Bis, 2A MORIN]</t>
+          <t xml:space="preserve"> &gt; ALGEBRA LINEARE ED ELEMENTI DI GEOMETRIA [H2 Bis, 2A MORIN]
+ &gt; INTRODUZIONE AL MACHINE LEARNING [H2 Bis, 5A]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1B]
- &gt; COMPUTABILITà, COMPLESSITà E LOGICA [H2 Bis, 2A MORIN]
- &gt; INTRODUZIONE AL MACHINE LEARNING [H3, 1A]</t>
+          <t xml:space="preserve"> &gt; ALGEBRA LINEARE ED ELEMENTI DI GEOMETRIA [H2 Bis, 2A MORIN]
+ &gt; INTRODUZIONE AL MACHINE LEARNING [H2 Bis, 5A]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1B]
- &gt; COMPUTABILITà, COMPLESSITà E LOGICA [H2 Bis, 2A MORIN]
- &gt; INTRODUZIONE AL MACHINE LEARNING [H3, 1A]</t>
+          <t xml:space="preserve"> &gt; ANALISI 1 [H3, 2B]
+ &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H3, 1B]</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1B]</t>
+          <t xml:space="preserve"> &gt; ANALISI 1 [H3, 2B]
+ &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H3, 1B]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -725,45 +716,53 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ANALISI 1 [H3, 1B]
- &gt; INFERENZA STATISTICA [H2 Bis, 3B]</t>
+          <t xml:space="preserve"> &gt; COMPUTABILITà, COMPLESSITà E LOGICA [H3, 2C]
+ &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H2 Bis, 5B]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ANALISI 1 [H3, 1B]
- &gt; INFERENZA STATISTICA [H2 Bis, 3B]</t>
+          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1B]
+ &gt; COMPUTABILITà, COMPLESSITà E LOGICA [H3, 2C]
+ &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H2 Bis, 5B]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; NESSUNA LEZIONE</t>
+          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1B]
+ &gt; COMPUTABILITà, COMPLESSITà E LOGICA [H3, 2C]
+ &gt; INTRODUZIONE ALL INTELLIGENZA ARTIFICIALE [H2 Bis, 5B]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; COMPUTABILITà, COMPLESSITà E LOGICA [H2 Bis, 3B]</t>
+          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1B]
+ &gt; COMPUTABILITà, COMPLESSITà E LOGICA [H3, 2C]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; COMPUTABILITà, COMPLESSITà E LOGICA [H2 Bis, 3B]</t>
+          <t xml:space="preserve"> &gt; INTRODUZIONE ALLA PROGRAMMAZIONE E LABORATORIO [H3, 1B]
+ &gt; COMPUTABILITà, COMPLESSITà E LOGICA [H3, 2C]</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ALGEBRA LINEARE ED ELEMENTI DI GEOMETRIA [H3, 2A]</t>
+          <t xml:space="preserve"> &gt; COMPUTABILITà, COMPLESSITà E LOGICA [H3, 2C]</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; ALGEBRA LINEARE ED ELEMENTI DI GEOMETRIA [H3, 2A]
- &gt; PROGRAMMAZIONE AVANZATA E PARALLELA [H2 Bis, 2A MORIN]</t>
+          <t xml:space="preserve"> &gt; ALGEBRA LINEARE ED ELEMENTI DI GEOMETRIA [H3, 1A]
+ &gt; INFERENZA STATISTICA [H3, 1C]
+ &gt; INTRODUZIONE AL MACHINE LEARNING [H3, 2C]</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> &gt; PROGRAMMAZIONE AVANZATA E PARALLELA [H2 Bis, 2A MORIN]</t>
+          <t xml:space="preserve"> &gt; ALGEBRA LINEARE ED ELEMENTI DI GEOMETRIA [H3, 1A]
+ &gt; INFERENZA STATISTICA [H3, 1C]
+ &gt; INTRODUZIONE AL MACHINE LEARNING [H3, 2C]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">

</xml_diff>